<commit_message>
Im making a template file for the script to help output discs like the toolbox
Im making a template file for the script to help output discs like the toolbox
it will eventually be like a catalogue which cant break, then the user can add the offsets and tolerancing based on their preferred way of making it
</commit_message>
<xml_diff>
--- a/App/cycloidal_parametric_design_sheet.xlsx
+++ b/App/cycloidal_parametric_design_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\CycloidialStudy\App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5171AEE1-0081-46C6-8B4A-BEFBE4B21C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940F3BC3-D79E-4BE8-9FD4-386D3F19A92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="18432" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DesignSheet" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,8 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">

</xml_diff>